<commit_message>
updated datos al dashboard 2024
</commit_message>
<xml_diff>
--- a/input/eitc_municipal_2023.xlsx
+++ b/input/eitc_municipal_2023.xlsx
@@ -1,15 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10421"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Documents/GitHub/Repos/Espacios-Abiertos/eitc-tableau/input/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9891E056-2CFB-EA40-987B-CBC6C5232E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -112,9 +131,6 @@
     <t>Aibonito</t>
   </si>
   <si>
-    <t>Anasco</t>
-  </si>
-  <si>
     <t>Arecibo</t>
   </si>
   <si>
@@ -127,9 +143,6 @@
     <t>Barranquitas</t>
   </si>
   <si>
-    <t>Bayamon</t>
-  </si>
-  <si>
     <t>Cabo Rojo</t>
   </si>
   <si>
@@ -139,15 +152,9 @@
     <t>Camuy</t>
   </si>
   <si>
-    <t>Canovanas</t>
-  </si>
-  <si>
     <t>Carolina</t>
   </si>
   <si>
-    <t>Catano</t>
-  </si>
-  <si>
     <t>Cayey</t>
   </si>
   <si>
@@ -163,9 +170,6 @@
     <t>Coamo</t>
   </si>
   <si>
-    <t>Comerio</t>
-  </si>
-  <si>
     <t>Corozal</t>
   </si>
   <si>
@@ -181,9 +185,6 @@
     <t>Florida</t>
   </si>
   <si>
-    <t>Guanica</t>
-  </si>
-  <si>
     <t>Guayama</t>
   </si>
   <si>
@@ -211,9 +212,6 @@
     <t>Jayuya</t>
   </si>
   <si>
-    <t>Juana Diaz</t>
-  </si>
-  <si>
     <t>Juncos</t>
   </si>
   <si>
@@ -223,30 +221,18 @@
     <t>Lares</t>
   </si>
   <si>
-    <t>Las Marias</t>
-  </si>
-  <si>
     <t>Las Piedras</t>
   </si>
   <si>
-    <t>Loiza</t>
-  </si>
-  <si>
     <t>Luquillo</t>
   </si>
   <si>
-    <t>Manati</t>
-  </si>
-  <si>
     <t>Maricao</t>
   </si>
   <si>
     <t>Maunabo</t>
   </si>
   <si>
-    <t>Mayaguez</t>
-  </si>
-  <si>
     <t>Moca</t>
   </si>
   <si>
@@ -268,39 +254,24 @@
     <t>Patillas</t>
   </si>
   <si>
-    <t>Penuelas</t>
-  </si>
-  <si>
     <t>Ponce</t>
   </si>
   <si>
     <t>Quebradillas</t>
   </si>
   <si>
-    <t>Rincon</t>
-  </si>
-  <si>
-    <t>Rio Grande</t>
-  </si>
-  <si>
     <t>Sabana Grande</t>
   </si>
   <si>
     <t>Salinas</t>
   </si>
   <si>
-    <t>San German</t>
-  </si>
-  <si>
     <t>San Juan</t>
   </si>
   <si>
     <t>San Lorenzo</t>
   </si>
   <si>
-    <t>San Sebastian</t>
-  </si>
-  <si>
     <t>Santa Isabel</t>
   </si>
   <si>
@@ -332,23 +303,76 @@
   </si>
   <si>
     <t>Yauco</t>
+  </si>
+  <si>
+    <t>Añasco</t>
+  </si>
+  <si>
+    <t>Bayamón</t>
+  </si>
+  <si>
+    <t>Canóvanas</t>
+  </si>
+  <si>
+    <t>Cataño</t>
+  </si>
+  <si>
+    <t>Comerío</t>
+  </si>
+  <si>
+    <t>Guánica</t>
+  </si>
+  <si>
+    <t>Juana Díaz</t>
+  </si>
+  <si>
+    <t>Las Marías</t>
+  </si>
+  <si>
+    <t>Loíza</t>
+  </si>
+  <si>
+    <t>Manatí</t>
+  </si>
+  <si>
+    <t>Mayagüez</t>
+  </si>
+  <si>
+    <t>Peñuelas</t>
+  </si>
+  <si>
+    <t>Rincón</t>
+  </si>
+  <si>
+    <t>Río Grande</t>
+  </si>
+  <si>
+    <t>San Germán</t>
+  </si>
+  <si>
+    <t>San Sebastián</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="#,##0;[Red]-#,##0"/>
-    <numFmt numFmtId="165" formatCode="#,##0.000;[Red]-#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000;[Red]\-#,##0.000"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
     </font>
   </fonts>
   <fills count="2">
@@ -371,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -382,63 +406,151 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf/>
+  <dxfs count="27">
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0;[Red]-#,##0"/>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Helvetica Neue"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="#,##0.000;[Red]-#,##0.000"/>
+      <numFmt numFmtId="165" formatCode="#,##0.000;[Red]\-#,##0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:AA80" totalsRowShown="0">
-  <autoFilter ref="A1:AA80"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Frame0" displayName="Frame0" ref="A1:AA80" totalsRowShown="0">
+  <autoFilter ref="A1:AA80" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="27">
-    <tableColumn id="1" name="Municipios" dataDxfId="0"/>
-    <tableColumn id="2" name="Año contributivo" dataDxfId="1"/>
-    <tableColumn id="3" name="Ingreso Bruto Ajustado - Casados" dataDxfId="1"/>
-    <tableColumn id="4" name="Planillas - Ingreso Bruto Ajustado - Casados" dataDxfId="1"/>
-    <tableColumn id="5" name="Ingreso Bruto Ajustado - Contribuyente Individual" dataDxfId="1"/>
-    <tableColumn id="6" name="Planillas - Ingreso Bruto Ajustado - Contribuyente Individual" dataDxfId="1"/>
-    <tableColumn id="7" name="Casados - Total Ingreso bruto ganado para la determinación del EITC" dataDxfId="1"/>
-    <tableColumn id="8" name="Planillas Casados - Total Ingreso bruto ganado para la determinación del EITC" dataDxfId="1"/>
-    <tableColumn id="9" name="Contribuyente Individual - Total Ingreso bruto ganado para la determinación del EITC" dataDxfId="1"/>
-    <tableColumn id="10" name="Planillas Contribuyente Individual - Total Ingreso bruto ganado para la determinación del EITC" dataDxfId="1"/>
-    <tableColumn id="11" name="Anejo CT: Ingresos Salarios" dataDxfId="1"/>
-    <tableColumn id="12" name="Planillas - Anejo CT: Ingresos Salarios" dataDxfId="1"/>
-    <tableColumn id="13" name="Anejo CT: Ingresos Pensión" dataDxfId="1"/>
-    <tableColumn id="14" name="Planillas - Anejo CT: Ingresos Pensión" dataDxfId="1"/>
-    <tableColumn id="15" name="Anejo CT: Ingresos Industria o Negocio" dataDxfId="1"/>
-    <tableColumn id="16" name="Planillas - Anejo CT: Ingresos Industria o Negocio" dataDxfId="1"/>
-    <tableColumn id="17" name="Anejo CT Total ingreso Bruto Ganado" dataDxfId="1"/>
-    <tableColumn id="18" name="Planillas - Anejo CT Total ingreso Bruto Ganado" dataDxfId="1"/>
-    <tableColumn id="19" name="Crédito por Trabajo - Casados" dataDxfId="1"/>
-    <tableColumn id="20" name="Planillas Casados - Crédito por Trabajo" dataDxfId="1"/>
-    <tableColumn id="21" name="Crédito por Trabajo - Contribuyente Individual" dataDxfId="1"/>
-    <tableColumn id="22" name="Planillas Contribuyente Individual - Crédito por Trabajo" dataDxfId="1"/>
-    <tableColumn id="23" name="Anejo CT Cantidad de dependientes cualificados" dataDxfId="1"/>
-    <tableColumn id="24" name="Planillas - Anejo CT Cantidad de dependientes cualificados" dataDxfId="1"/>
-    <tableColumn id="25" name="Crédito por Trabajo - Total" dataDxfId="1"/>
-    <tableColumn id="26" name="Planillas Total - Crédito por Trabajo" dataDxfId="1"/>
-    <tableColumn id="27" name="Crédito por Trabajo - Promedio" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Municipios" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Año contributivo" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Ingreso Bruto Ajustado - Casados" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Planillas - Ingreso Bruto Ajustado - Casados" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Ingreso Bruto Ajustado - Contribuyente Individual" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Planillas - Ingreso Bruto Ajustado - Contribuyente Individual" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Casados - Total Ingreso bruto ganado para la determinación del EITC" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Planillas Casados - Total Ingreso bruto ganado para la determinación del EITC" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Contribuyente Individual - Total Ingreso bruto ganado para la determinación del EITC" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Planillas Contribuyente Individual - Total Ingreso bruto ganado para la determinación del EITC" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Anejo CT: Ingresos Salarios" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Planillas - Anejo CT: Ingresos Salarios" dataDxfId="16"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Anejo CT: Ingresos Pensión" dataDxfId="15"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Planillas - Anejo CT: Ingresos Pensión" dataDxfId="14"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Anejo CT: Ingresos Industria o Negocio" dataDxfId="13"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Planillas - Anejo CT: Ingresos Industria o Negocio" dataDxfId="12"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Anejo CT Total ingreso Bruto Ganado" dataDxfId="11"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Planillas - Anejo CT Total ingreso Bruto Ganado" dataDxfId="10"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Crédito por Trabajo - Casados" dataDxfId="9"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Planillas Casados - Crédito por Trabajo" dataDxfId="8"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Crédito por Trabajo - Contribuyente Individual" dataDxfId="7"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Planillas Contribuyente Individual - Crédito por Trabajo" dataDxfId="6"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Anejo CT Cantidad de dependientes cualificados" dataDxfId="5"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Planillas - Anejo CT Cantidad de dependientes cualificados" dataDxfId="4"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Crédito por Trabajo - Total" dataDxfId="3"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Planillas Total - Crédito por Trabajo" dataDxfId="2"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Crédito por Trabajo - Promedio" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -476,7 +588,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -510,6 +622,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -544,9 +657,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -719,14 +833,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -809,8 +928,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="2">
@@ -892,8 +1011,8 @@
         <v>1946.092315369262</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="2">
@@ -975,8 +1094,8 @@
         <v>1926.817218869319</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="2">
@@ -1055,11 +1174,11 @@
         <v>10469</v>
       </c>
       <c r="AA4" s="3">
-        <v>1950.077180246442</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27">
-      <c r="A5" s="1" t="s">
+        <v>1950.0771802464419</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="2">
@@ -1138,11 +1257,11 @@
         <v>4690</v>
       </c>
       <c r="AA5" s="3">
-        <v>1884.185501066098</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27">
-      <c r="A6" s="1" t="s">
+        <v>1884.1855010660979</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="2">
@@ -1221,12 +1340,12 @@
         <v>5180</v>
       </c>
       <c r="AA6" s="3">
-        <v>1861.442277992278</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27">
-      <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>1861.4422779922779</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="B7" s="2">
         <v>2023</v>
@@ -1307,9 +1426,9 @@
         <v>1881.337957124842</v>
       </c>
     </row>
-    <row r="8" spans="1:27">
-      <c r="A8" s="1" t="s">
-        <v>33</v>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="B8" s="2">
         <v>2023</v>
@@ -1387,12 +1506,12 @@
         <v>17562</v>
       </c>
       <c r="AA8" s="3">
-        <v>1869.986049424895</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27">
-      <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>1869.9860494248951</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="B9" s="2">
         <v>2023</v>
@@ -1470,12 +1589,12 @@
         <v>3366</v>
       </c>
       <c r="AA9" s="3">
-        <v>1918.805407011289</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27">
-      <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>1918.8054070112889</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="B10" s="2">
         <v>2023</v>
@@ -1556,9 +1675,9 @@
         <v>1932.781908036098</v>
       </c>
     </row>
-    <row r="11" spans="1:27">
-      <c r="A11" s="1" t="s">
-        <v>36</v>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="B11" s="2">
         <v>2023</v>
@@ -1636,12 +1755,12 @@
         <v>6038</v>
       </c>
       <c r="AA11" s="3">
-        <v>2090.35607817158</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27">
-      <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>2090.3560781715801</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="B12" s="2">
         <v>2023</v>
@@ -1722,9 +1841,9 @@
         <v>1773.514445505388</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
-      <c r="A13" s="1" t="s">
-        <v>38</v>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="B13" s="2">
         <v>2023</v>
@@ -1802,12 +1921,12 @@
         <v>8735</v>
       </c>
       <c r="AA13" s="3">
-        <v>1822.842243846594</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27">
-      <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>1822.8422438465941</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="B14" s="2">
         <v>2023</v>
@@ -1888,9 +2007,9 @@
         <v>1806.645281944953</v>
       </c>
     </row>
-    <row r="15" spans="1:27">
-      <c r="A15" s="1" t="s">
-        <v>40</v>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="B15" s="2">
         <v>2023</v>
@@ -1968,12 +2087,12 @@
         <v>6461</v>
       </c>
       <c r="AA15" s="3">
-        <v>1936.964401795388</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27">
-      <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>1936.9644017953881</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="B16" s="2">
         <v>2023</v>
@@ -2051,12 +2170,12 @@
         <v>9238</v>
       </c>
       <c r="AA16" s="3">
-        <v>1892.686512232085</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27">
-      <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>1892.6865122320851</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="B17" s="2">
         <v>2023</v>
@@ -2137,9 +2256,9 @@
         <v>1761.281925866773</v>
       </c>
     </row>
-    <row r="18" spans="1:27">
-      <c r="A18" s="1" t="s">
-        <v>43</v>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="B18" s="2">
         <v>2023</v>
@@ -2220,9 +2339,9 @@
         <v>1930.653405405405</v>
       </c>
     </row>
-    <row r="19" spans="1:27">
-      <c r="A19" s="1" t="s">
-        <v>44</v>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B19" s="2">
         <v>2023</v>
@@ -2300,12 +2419,12 @@
         <v>8949</v>
       </c>
       <c r="AA19" s="3">
-        <v>1902.388982009163</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27">
-      <c r="A20" s="1" t="s">
-        <v>45</v>
+        <v>1902.3889820091631</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="B20" s="2">
         <v>2023</v>
@@ -2383,12 +2502,12 @@
         <v>2332</v>
       </c>
       <c r="AA20" s="3">
-        <v>1898.037735849057</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27">
-      <c r="A21" s="1" t="s">
-        <v>46</v>
+        <v>1898.0377358490571</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="B21" s="2">
         <v>2023</v>
@@ -2466,12 +2585,12 @@
         <v>3641</v>
       </c>
       <c r="AA21" s="3">
-        <v>2043.488602032409</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27">
-      <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>2043.4886020324091</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="B22" s="2">
         <v>2023</v>
@@ -2552,9 +2671,9 @@
         <v>1945.889055064582</v>
       </c>
     </row>
-    <row r="23" spans="1:27">
-      <c r="A23" s="1" t="s">
-        <v>48</v>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="B23" s="2">
         <v>2023</v>
@@ -2635,9 +2754,9 @@
         <v>1947.241079075078</v>
       </c>
     </row>
-    <row r="24" spans="1:27">
-      <c r="A24" s="1" t="s">
-        <v>49</v>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="B24" s="2">
         <v>2023</v>
@@ -2715,12 +2834,12 @@
         <v>3501</v>
       </c>
       <c r="AA24" s="3">
-        <v>2017.724364467295</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27">
-      <c r="A25" s="1" t="s">
-        <v>50</v>
+        <v>2017.7243644672949</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="B25" s="2">
         <v>2023</v>
@@ -2798,12 +2917,12 @@
         <v>7159</v>
       </c>
       <c r="AA25" s="3">
-        <v>2074.758066769102</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27">
-      <c r="A26" s="1" t="s">
-        <v>51</v>
+        <v>2074.7580667691018</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="B26" s="2">
         <v>2023</v>
@@ -2884,9 +3003,9 @@
         <v>1744.767213114754</v>
       </c>
     </row>
-    <row r="27" spans="1:27">
-      <c r="A27" s="1" t="s">
-        <v>52</v>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="B27" s="2">
         <v>2023</v>
@@ -2964,12 +3083,12 @@
         <v>6138</v>
       </c>
       <c r="AA27" s="3">
-        <v>1866.181981101336</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27">
-      <c r="A28" s="1" t="s">
-        <v>53</v>
+        <v>1866.1819811013361</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="B28" s="2">
         <v>2023</v>
@@ -3050,9 +3169,9 @@
         <v>1876.345503116652</v>
       </c>
     </row>
-    <row r="29" spans="1:27">
-      <c r="A29" s="1" t="s">
-        <v>54</v>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="B29" s="2">
         <v>2023</v>
@@ -3133,9 +3252,9 @@
         <v>2046.669902912621</v>
       </c>
     </row>
-    <row r="30" spans="1:27">
-      <c r="A30" s="1" t="s">
-        <v>55</v>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="B30" s="2">
         <v>2023</v>
@@ -3213,12 +3332,12 @@
         <v>3006</v>
       </c>
       <c r="AA30" s="3">
-        <v>1949.756154357951</v>
-      </c>
-    </row>
-    <row r="31" spans="1:27">
-      <c r="A31" s="1" t="s">
-        <v>56</v>
+        <v>1949.7561543579509</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="B31" s="2">
         <v>2023</v>
@@ -3296,12 +3415,12 @@
         <v>8139</v>
       </c>
       <c r="AA31" s="3">
-        <v>1896.994225334808</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27">
-      <c r="A32" s="1" t="s">
-        <v>57</v>
+        <v>1896.9942253348081</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="B32" s="2">
         <v>2023</v>
@@ -3379,12 +3498,12 @@
         <v>4056</v>
       </c>
       <c r="AA32" s="3">
-        <v>1880.931706114398</v>
-      </c>
-    </row>
-    <row r="33" spans="1:27">
-      <c r="A33" s="1" t="s">
-        <v>58</v>
+        <v>1880.9317061143979</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="B33" s="2">
         <v>2023</v>
@@ -3462,12 +3581,12 @@
         <v>13167</v>
       </c>
       <c r="AA33" s="3">
-        <v>1703.610693400167</v>
-      </c>
-    </row>
-    <row r="34" spans="1:27">
-      <c r="A34" s="1" t="s">
-        <v>59</v>
+        <v>1703.6106934001671</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="B34" s="2">
         <v>2023</v>
@@ -3545,12 +3664,12 @@
         <v>7042</v>
       </c>
       <c r="AA34" s="3">
-        <v>1844.353166714002</v>
-      </c>
-    </row>
-    <row r="35" spans="1:27">
-      <c r="A35" s="1" t="s">
-        <v>60</v>
+        <v>1844.3531667140021</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="B35" s="2">
         <v>2023</v>
@@ -3628,12 +3747,12 @@
         <v>6733</v>
       </c>
       <c r="AA35" s="3">
-        <v>1957.189811376801</v>
-      </c>
-    </row>
-    <row r="36" spans="1:27">
-      <c r="A36" s="1" t="s">
-        <v>61</v>
+        <v>1957.1898113768009</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="B36" s="2">
         <v>2023</v>
@@ -3711,12 +3830,12 @@
         <v>3526</v>
       </c>
       <c r="AA36" s="3">
-        <v>1793.416619398752</v>
-      </c>
-    </row>
-    <row r="37" spans="1:27">
-      <c r="A37" s="1" t="s">
-        <v>62</v>
+        <v>1793.4166193987519</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="B37" s="2">
         <v>2023</v>
@@ -3794,12 +3913,12 @@
         <v>10176</v>
       </c>
       <c r="AA37" s="3">
-        <v>1917.89465408805</v>
-      </c>
-    </row>
-    <row r="38" spans="1:27">
-      <c r="A38" s="1" t="s">
-        <v>63</v>
+        <v>1917.8946540880499</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="B38" s="2">
         <v>2023</v>
@@ -3877,12 +3996,12 @@
         <v>8101</v>
       </c>
       <c r="AA38" s="3">
-        <v>1924.278484137761</v>
-      </c>
-    </row>
-    <row r="39" spans="1:27">
-      <c r="A39" s="1" t="s">
-        <v>64</v>
+        <v>1924.2784841377611</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B39" s="2">
         <v>2023</v>
@@ -3963,9 +4082,9 @@
         <v>1945.050307107341</v>
       </c>
     </row>
-    <row r="40" spans="1:27">
-      <c r="A40" s="1" t="s">
-        <v>65</v>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>96</v>
       </c>
       <c r="B40" s="2">
         <v>2023</v>
@@ -4043,12 +4162,12 @@
         <v>9055</v>
       </c>
       <c r="AA40" s="3">
-        <v>1956.764329099945</v>
-      </c>
-    </row>
-    <row r="41" spans="1:27">
-      <c r="A41" s="1" t="s">
-        <v>66</v>
+        <v>1956.7643290999449</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="B41" s="2">
         <v>2023</v>
@@ -4126,12 +4245,12 @@
         <v>7078</v>
       </c>
       <c r="AA41" s="3">
-        <v>1943.526137326929</v>
-      </c>
-    </row>
-    <row r="42" spans="1:27">
-      <c r="A42" s="1" t="s">
-        <v>67</v>
+        <v>1943.5261373269291</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="B42" s="2">
         <v>2023</v>
@@ -4212,9 +4331,9 @@
         <v>1915.068848996832</v>
       </c>
     </row>
-    <row r="43" spans="1:27">
-      <c r="A43" s="1" t="s">
-        <v>68</v>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="B43" s="2">
         <v>2023</v>
@@ -4295,9 +4414,9 @@
         <v>1937.74227865477</v>
       </c>
     </row>
-    <row r="44" spans="1:27">
-      <c r="A44" s="1" t="s">
-        <v>69</v>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="B44" s="2">
         <v>2023</v>
@@ -4375,12 +4494,12 @@
         <v>1997</v>
       </c>
       <c r="AA44" s="3">
-        <v>2034.362043064597</v>
-      </c>
-    </row>
-    <row r="45" spans="1:27">
-      <c r="A45" s="1" t="s">
-        <v>70</v>
+        <v>2034.3620430645969</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="B45" s="2">
         <v>2023</v>
@@ -4461,9 +4580,9 @@
         <v>1924.254062262718</v>
       </c>
     </row>
-    <row r="46" spans="1:27">
-      <c r="A46" s="1" t="s">
-        <v>71</v>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="B46" s="2">
         <v>2023</v>
@@ -4544,9 +4663,9 @@
         <v>1937.758766768651</v>
       </c>
     </row>
-    <row r="47" spans="1:27">
-      <c r="A47" s="1" t="s">
-        <v>72</v>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="B47" s="2">
         <v>2023</v>
@@ -4627,9 +4746,9 @@
         <v>1839.007061713233</v>
       </c>
     </row>
-    <row r="48" spans="1:27">
-      <c r="A48" s="1" t="s">
-        <v>73</v>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="B48" s="2">
         <v>2023</v>
@@ -4710,9 +4829,9 @@
         <v>1965.259153094463</v>
       </c>
     </row>
-    <row r="49" spans="1:27">
-      <c r="A49" s="1" t="s">
-        <v>74</v>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="B49" s="2">
         <v>2023</v>
@@ -4793,9 +4912,9 @@
         <v>1832.904295403165</v>
       </c>
     </row>
-    <row r="50" spans="1:27">
-      <c r="A50" s="1" t="s">
-        <v>75</v>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="B50" s="2">
         <v>2023</v>
@@ -4876,9 +4995,9 @@
         <v>1888.355221158231</v>
       </c>
     </row>
-    <row r="51" spans="1:27">
-      <c r="A51" s="1" t="s">
-        <v>76</v>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="B51" s="2">
         <v>2023</v>
@@ -4959,9 +5078,9 @@
         <v>1857.874179506668</v>
       </c>
     </row>
-    <row r="52" spans="1:27">
-      <c r="A52" s="1" t="s">
-        <v>77</v>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="B52" s="2">
         <v>2023</v>
@@ -5042,9 +5161,9 @@
         <v>1994.524195591589</v>
       </c>
     </row>
-    <row r="53" spans="1:27">
-      <c r="A53" s="1" t="s">
-        <v>78</v>
+    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="B53" s="2">
         <v>2023</v>
@@ -5125,9 +5244,9 @@
         <v>2011.623017902813</v>
       </c>
     </row>
-    <row r="54" spans="1:27">
-      <c r="A54" s="1" t="s">
-        <v>79</v>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="B54" s="2">
         <v>2023</v>
@@ -5208,9 +5327,9 @@
         <v>2045.408521853723</v>
       </c>
     </row>
-    <row r="55" spans="1:27">
-      <c r="A55" s="1" t="s">
-        <v>80</v>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="B55" s="2">
         <v>2023</v>
@@ -5291,9 +5410,9 @@
         <v>2027.557937039518</v>
       </c>
     </row>
-    <row r="56" spans="1:27">
-      <c r="A56" s="1" t="s">
-        <v>81</v>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="B56" s="2">
         <v>2023</v>
@@ -5371,12 +5490,12 @@
         <v>4391</v>
       </c>
       <c r="AA56" s="3">
-        <v>2068.774083352312</v>
-      </c>
-    </row>
-    <row r="57" spans="1:27">
+        <v>2068.7740833523121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B57" s="2">
         <v>2023</v>
@@ -5457,9 +5576,9 @@
         <v>1775.489126280733</v>
       </c>
     </row>
-    <row r="58" spans="1:27">
-      <c r="A58" s="1" t="s">
-        <v>83</v>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="B58" s="2">
         <v>2023</v>
@@ -5537,12 +5656,12 @@
         <v>3147</v>
       </c>
       <c r="AA58" s="3">
-        <v>1927.992373689228</v>
-      </c>
-    </row>
-    <row r="59" spans="1:27">
-      <c r="A59" s="1" t="s">
-        <v>84</v>
+        <v>1927.9923736892281</v>
+      </c>
+    </row>
+    <row r="59" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="B59" s="2">
         <v>2023</v>
@@ -5623,9 +5742,9 @@
         <v>2004.519788359788</v>
       </c>
     </row>
-    <row r="60" spans="1:27">
-      <c r="A60" s="1" t="s">
-        <v>85</v>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="B60" s="2">
         <v>2023</v>
@@ -5703,12 +5822,12 @@
         <v>29948</v>
       </c>
       <c r="AA60" s="3">
-        <v>1917.662281287565</v>
-      </c>
-    </row>
-    <row r="61" spans="1:27">
-      <c r="A61" s="1" t="s">
-        <v>86</v>
+        <v>1917.6622812875651</v>
+      </c>
+    </row>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="B61" s="2">
         <v>2023</v>
@@ -5786,12 +5905,12 @@
         <v>5324</v>
       </c>
       <c r="AA61" s="3">
-        <v>1950.74173553719</v>
-      </c>
-    </row>
-    <row r="62" spans="1:27">
-      <c r="A62" s="1" t="s">
-        <v>87</v>
+        <v>1950.7417355371899</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="B62" s="2">
         <v>2023</v>
@@ -5869,12 +5988,12 @@
         <v>2763</v>
       </c>
       <c r="AA62" s="3">
-        <v>1864.591024249005</v>
-      </c>
-    </row>
-    <row r="63" spans="1:27">
-      <c r="A63" s="1" t="s">
-        <v>88</v>
+        <v>1864.5910242490049</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
+        <v>103</v>
       </c>
       <c r="B63" s="2">
         <v>2023</v>
@@ -5952,12 +6071,12 @@
         <v>9638</v>
       </c>
       <c r="AA63" s="3">
-        <v>1882.708653247562</v>
-      </c>
-    </row>
-    <row r="64" spans="1:27">
-      <c r="A64" s="1" t="s">
-        <v>89</v>
+        <v>1882.7086532475621</v>
+      </c>
+    </row>
+    <row r="64" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="B64" s="2">
         <v>2023</v>
@@ -6038,9 +6157,9 @@
         <v>1923.697249632585</v>
       </c>
     </row>
-    <row r="65" spans="1:27">
-      <c r="A65" s="1" t="s">
-        <v>90</v>
+    <row r="65" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="B65" s="2">
         <v>2023</v>
@@ -6118,12 +6237,12 @@
         <v>4073</v>
       </c>
       <c r="AA65" s="3">
-        <v>1888.804321139209</v>
-      </c>
-    </row>
-    <row r="66" spans="1:27">
-      <c r="A66" s="1" t="s">
-        <v>91</v>
+        <v>1888.8043211392089</v>
+      </c>
+    </row>
+    <row r="66" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="B66" s="2">
         <v>2023</v>
@@ -6204,9 +6323,9 @@
         <v>1867.854139715394</v>
       </c>
     </row>
-    <row r="67" spans="1:27">
-      <c r="A67" s="1" t="s">
-        <v>92</v>
+    <row r="67" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="B67" s="2">
         <v>2023</v>
@@ -6287,9 +6406,9 @@
         <v>1752.370472129048</v>
       </c>
     </row>
-    <row r="68" spans="1:27">
-      <c r="A68" s="1" t="s">
-        <v>93</v>
+    <row r="68" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="B68" s="2">
         <v>2023</v>
@@ -6370,9 +6489,9 @@
         <v>1938.729125667697</v>
       </c>
     </row>
-    <row r="69" spans="1:27">
-      <c r="A69" s="1" t="s">
-        <v>94</v>
+    <row r="69" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="B69" s="2">
         <v>2023</v>
@@ -6450,12 +6569,12 @@
         <v>8346</v>
       </c>
       <c r="AA69" s="3">
-        <v>1955.03474718428</v>
-      </c>
-    </row>
-    <row r="70" spans="1:27">
-      <c r="A70" s="1" t="s">
-        <v>95</v>
+        <v>1955.0347471842799</v>
+      </c>
+    </row>
+    <row r="70" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="B70" s="2">
         <v>2023</v>
@@ -6536,9 +6655,9 @@
         <v>1899.643548006605</v>
       </c>
     </row>
-    <row r="71" spans="1:27">
-      <c r="A71" s="1" t="s">
-        <v>96</v>
+    <row r="71" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A71" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="B71" s="2">
         <v>2023</v>
@@ -6619,9 +6738,9 @@
         <v>1890.501498252039</v>
       </c>
     </row>
-    <row r="72" spans="1:27">
-      <c r="A72" s="1" t="s">
-        <v>97</v>
+    <row r="72" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="B72" s="2">
         <v>2023</v>
@@ -6699,12 +6818,12 @@
         <v>15085</v>
       </c>
       <c r="AA72" s="3">
-        <v>1809.886443486908</v>
-      </c>
-    </row>
-    <row r="73" spans="1:27">
-      <c r="A73" s="1" t="s">
-        <v>98</v>
+        <v>1809.8864434869081</v>
+      </c>
+    </row>
+    <row r="73" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="B73" s="2">
         <v>2023</v>
@@ -6785,9 +6904,9 @@
         <v>1766.257216103304</v>
       </c>
     </row>
-    <row r="74" spans="1:27">
-      <c r="A74" s="1" t="s">
-        <v>99</v>
+    <row r="74" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="B74" s="2">
         <v>2023</v>
@@ -6865,12 +6984,12 @@
         <v>5305</v>
       </c>
       <c r="AA74" s="3">
-        <v>1954.482940622055</v>
-      </c>
-    </row>
-    <row r="75" spans="1:27">
-      <c r="A75" s="1" t="s">
-        <v>100</v>
+        <v>1954.4829406220549</v>
+      </c>
+    </row>
+    <row r="75" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="B75" s="2">
         <v>2023</v>
@@ -6948,12 +7067,12 @@
         <v>6459</v>
       </c>
       <c r="AA75" s="3">
-        <v>2001.328843474222</v>
-      </c>
-    </row>
-    <row r="76" spans="1:27">
-      <c r="A76" s="1" t="s">
-        <v>101</v>
+        <v>2001.3288434742219</v>
+      </c>
+    </row>
+    <row r="76" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="B76" s="2">
         <v>2023</v>
@@ -7031,12 +7150,12 @@
         <v>10594</v>
       </c>
       <c r="AA76" s="3">
-        <v>1941.626581083632</v>
-      </c>
-    </row>
-    <row r="77" spans="1:27">
-      <c r="A77" s="1" t="s">
-        <v>102</v>
+        <v>1941.6265810836319</v>
+      </c>
+    </row>
+    <row r="77" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="B77" s="2">
         <v>2023</v>
@@ -7114,12 +7233,12 @@
         <v>1156</v>
       </c>
       <c r="AA77" s="3">
-        <v>1936.614186851211</v>
-      </c>
-    </row>
-    <row r="78" spans="1:27">
-      <c r="A78" s="1" t="s">
-        <v>103</v>
+        <v>1936.6141868512109</v>
+      </c>
+    </row>
+    <row r="78" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A78" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="B78" s="2">
         <v>2023</v>
@@ -7200,9 +7319,9 @@
         <v>2061.869901812689</v>
       </c>
     </row>
-    <row r="79" spans="1:27">
-      <c r="A79" s="1" t="s">
-        <v>104</v>
+    <row r="79" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A79" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="B79" s="2">
         <v>2023</v>
@@ -7283,9 +7402,9 @@
         <v>1947.912861682556</v>
       </c>
     </row>
-    <row r="80" spans="1:27">
-      <c r="A80" s="1" t="s">
-        <v>105</v>
+    <row r="80" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A80" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="B80" s="2">
         <v>2023</v>

</xml_diff>